<commit_message>
Updated the formula example
</commit_message>
<xml_diff>
--- a/examples/example3.xlsx
+++ b/examples/example3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://informatica-my.sharepoint.com/personal/jbowring_informatica_com/Documents/_My Documents/Coding/Windows/Excel/Xml2Xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbowring\OneDrive - Informatica\_My Documents\Coding\Windows\Excel\Xml2Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_4005CDA74312137A86AD34418B49D9484606EEC4" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A0BF154B-6596-4D26-B67F-347425540F29}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D455DBAC-140A-4336-ADE2-DB7688B383BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -97,17 +97,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,33 +126,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,10 +447,10 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.109375" bestFit="1" customWidth="1"/>
@@ -486,91 +459,91 @@
     <col min="5" max="5" width="31.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="10" t="str">
+      <c r="E2" s="1" t="str">
         <f>A2&amp;" - "&amp;B2</f>
         <v>Everyday Italian - Giada De Laurentiis</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="2">
         <f>C2 * D2</f>
         <v>60150</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="16" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="20" t="str">
+      <c r="E4" s="1" t="str">
         <f>UPPER(A2)</f>
         <v>EVERYDAY ITALIAN</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="25" t="str">
+      <c r="E5" s="1" t="str">
         <f>LOWER(B2)</f>
         <v>giada de laurentiis</v>
       </c>

</xml_diff>